<commit_message>
model built. back off to a little data processing
</commit_message>
<xml_diff>
--- a/categories_names.xlsx
+++ b/categories_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YizhiZhang\Documents\GitHub\CreditRiskPractice\CreditRiskDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E98F182-5F97-44EA-8FF8-D3C212DA91BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4E833C-8553-4B5D-B534-1E0143226FFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2610" windowWidth="17280" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15015" yWindow="2430" windowWidth="17280" windowHeight="12345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of dummy variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="249">
   <si>
     <t>Always keeps the category with the worst credit risk as a reference category</t>
   </si>
@@ -175,9 +175,6 @@
     <t>'annual_inc:&gt;140K'</t>
   </si>
   <si>
-    <t>'mths_since_last_delinq:Missing'</t>
-  </si>
-  <si>
     <t>mths_since_last_delinq:Missing'</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>'mths_since_issue_d:&gt;84'</t>
   </si>
   <si>
-    <t>'mths_since_earliest_cr_line:&lt;140'</t>
-  </si>
-  <si>
     <t>mths_since_earliest_cr_line:&lt;140'</t>
   </si>
   <si>
@@ -353,6 +347,432 @@
   </si>
   <si>
     <t>'total_rev_hi_lim:&gt;92K'</t>
+  </si>
+  <si>
+    <t>'dti:&lt;4'</t>
+  </si>
+  <si>
+    <t>'dti:4-8'</t>
+  </si>
+  <si>
+    <t>'dti:8-12'</t>
+  </si>
+  <si>
+    <t>'dti:12-13.6'</t>
+  </si>
+  <si>
+    <t>'dti:13.6-16.8'</t>
+  </si>
+  <si>
+    <t>'dti:16.8-20.8'</t>
+  </si>
+  <si>
+    <t>'dti:20.8-24'</t>
+  </si>
+  <si>
+    <t>'dti:24-28'</t>
+  </si>
+  <si>
+    <t>'dti:&gt;28'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:Missing'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:0-4.8'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:4.8-24.2'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:24.2-36.3'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:36.3-50.8'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:50.8-67.8'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:67.8-80'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:80-84.7'</t>
+  </si>
+  <si>
+    <t>'mths_since_last_record:&gt;84.7'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:A', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:B', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:C', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:D', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:E', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:F', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grade:G', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'home_ownership:RENT_OTHER_NONE_ANY', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'home_ownership:OWN', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'home_ownership:MORTGAGE', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:ND_NE_IA_NV_FL_HI_AL', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:WV_NH_WY_DC_ME_ID', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:NM_VA', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:NY', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:OK_TN_MO_LA_MD_NC', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:CA', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:UT_KY_AZ_NJ', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:AR_MI_PA_OH_MN', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:RI_MA_DE_SD_IN', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:GA_WA_OR', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:WI_MT', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:IL_CT', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'addr_state:KS_SC_CO_VT_AK_MS', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'purpose:smabus_edu_mov_hou_oth', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'purpose:reen_med_wed_vac', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'purpose:debt_consolidation', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'purpose:hom_maj_car', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'purpose:credit_card', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'verification_status:Not Verified', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'verification_status:Source Verified', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'verification_status:Verified', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'initial_list_status:f', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'initial_list_status:w', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'term:36', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'term:60', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:1', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:2-4', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:5-6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:7-9', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'emp_length:10', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'int_rate:&lt;9.548', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'int_rate:9.548-12.025', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'int_rate:12.025-15.74', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'int_rate:15.75-20.281', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'int_rate:&gt;20.281', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:&lt;20K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:20K-30K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:30K-40K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:40K-50K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:50K-60K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:60K-70K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:70K-80K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:80K-90K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:90K-100K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:100K-120K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:120K-140K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'annual_inc:&gt;140K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_delinq:Missing', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_delinq:0-3', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_delinq:4-30', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_delinq:&gt;=57', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_delinq:31-56', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d::&lt;38', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'mths_since_issue_d:38-39', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:40-41', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:42-48', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mths_since_issue_d:49-52', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:53-64', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:65-84', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:&gt;84', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:&lt;140', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:141-164', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:165-247', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:248-270', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:271-352', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_earliest_cr_line:&gt;352', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'delinq_2yrs:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'delinq_2yrs:1-3', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'delinq_2yrs:&gt;=4', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'inq_last_6mths:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'inq_last_6mths:1-2', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'inq_last_6mths:3-6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'inq_last_6mths:&gt;6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:1-3', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:4-12', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:13-22', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:23-25', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:26-30', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'open_acc:&gt;30', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pub_rec:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pub_rec:1-2', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pub_rec:3-6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pub_rec:&gt;6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_acc:&lt;=9', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_acc:10-21', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_acc:22-33', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_acc:34-51', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_acc:&gt;51', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'acc_now_delinq:0', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'acc_now_delinq:&gt;=1', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_rev_hi_lim:&lt;36K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_rev_hi_lim:36K-56K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_rev_hi_lim:56K-92K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'total_rev_hi_lim:&gt;92K', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:&lt;4', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:4-8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:8-12', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:12-13.6', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:13.6-16.8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:16.8-20.8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:20.8-24', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:24-28', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dti:&gt;28', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:Missing', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:0-4.8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:4.8-24.2', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:24.2-36.3', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:36.3-50.8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:50.8-67.8', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:67.8-80', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:80-84.7', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_last_record:&gt;84.7', </t>
   </si>
 </sst>
 </file>
@@ -399,13 +819,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -686,542 +1111,1007 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A106"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="G1" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="G2" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="G3" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="G4" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="G5" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="G6" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="G7" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="G8" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="G9" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="G10" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="G11" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="G12" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="G13" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="G14" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="G15" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="G16" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="G17" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="G18" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="G19" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="G20" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="G21" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="G22" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="G23" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+      <c r="G25" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="G26" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="G27" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+      <c r="G28" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="G29" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+      <c r="G30" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+      <c r="G31" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="G32" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="G33" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="G34" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="G35" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="G36" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="G37" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="G38" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="G39" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="G40" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="G41" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="G42" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="G43" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="G44" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="G45" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="G46" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="G47" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="G48" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="G49" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="G50" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="G51" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="G52" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="G53" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="G54" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="G55" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="G56" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="G57" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="G58" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
+      <c r="G60" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
+      <c r="G61" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
+      <c r="G62" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="G63" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+      <c r="G65" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
+      <c r="G66" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="2" t="s">
+      <c r="G67" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+      <c r="G68" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+      <c r="G69" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+      <c r="G70" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+      <c r="G71" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="2" t="s">
+      <c r="G72" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+      <c r="G74" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+      <c r="G75" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
+      <c r="G76" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+      <c r="G77" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
+      <c r="G78" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
+      <c r="G79" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
+      <c r="G80" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
+      <c r="G81" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
+      <c r="G82" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="2" t="s">
+      <c r="G83" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
+      <c r="G84" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
+      <c r="G85" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
+      <c r="G86" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
+      <c r="G87" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="2" t="s">
+      <c r="G88" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
+      <c r="G89" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
+      <c r="G90" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
+      <c r="G91" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
+      <c r="G92" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
+      <c r="G93" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
+      <c r="G94" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
+      <c r="G95" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
+      <c r="G96" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
+      <c r="G97" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+      <c r="G98" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
+      <c r="G99" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
+      <c r="G100" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
+      <c r="G101" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
+      <c r="G102" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
+      <c r="G103" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
+      <c r="G104" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+      <c r="G105" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
+      <c r="G106" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
+      <c r="G107" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
         <v>108</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -1232,10 +2122,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4B0F96-FC90-42AD-8F1F-BCD27F5832B3}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1247,102 +2137,112 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="A5" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>55</v>
+      <c r="A6" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>60</v>
+      <c r="A7" s="6" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>63</v>
+      <c r="A8" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>25</v>
+      <c r="A9" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>36</v>
+      <c r="A11" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>37</v>
+      <c r="A12" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>49</v>
+      <c r="A13" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>72</v>
+      <c r="A14" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
-        <v>73</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>82</v>
+      <c r="A16" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>86</v>
+      <c r="A17" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>87</v>
+      <c r="A18" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>94</v>
+      <c r="A19" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>98</v>
+      <c r="A20" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>104</v>
+      <c r="A21" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>105</v>
+      <c r="A22" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quick update about model fit
</commit_message>
<xml_diff>
--- a/categories_names.xlsx
+++ b/categories_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YizhiZhang\Documents\GitHub\CreditRiskPractice\CreditRiskDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4E833C-8553-4B5D-B534-1E0143226FFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A029281-BD20-4766-9D88-57F817D19906}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15015" yWindow="2430" windowWidth="17280" windowHeight="12345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of dummy variables" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t xml:space="preserve"> 'mths_since_issue_d::&lt;38', </t>
   </si>
   <si>
-    <t xml:space="preserve">  'mths_since_issue_d:38-39', </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 'mths_since_issue_d:40-41', </t>
   </si>
   <si>
@@ -773,6 +770,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 'mths_since_last_record:&gt;84.7', </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'mths_since_issue_d:38-39', </t>
   </si>
 </sst>
 </file>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,7 +1639,7 @@
         <v>65</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1647,7 +1647,7 @@
         <v>66</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1655,7 +1655,7 @@
         <v>67</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1663,7 +1663,7 @@
         <v>68</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1671,7 +1671,7 @@
         <v>69</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1679,7 +1679,7 @@
         <v>70</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -1687,7 +1687,7 @@
         <v>71</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -1695,7 +1695,7 @@
         <v>72</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -1703,7 +1703,7 @@
         <v>73</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -1711,7 +1711,7 @@
         <v>74</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -1719,7 +1719,7 @@
         <v>75</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -1727,7 +1727,7 @@
         <v>76</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -1735,7 +1735,7 @@
         <v>77</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -1743,7 +1743,7 @@
         <v>78</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -1751,7 +1751,7 @@
         <v>79</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -1759,7 +1759,7 @@
         <v>80</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -1767,7 +1767,7 @@
         <v>81</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -1775,7 +1775,7 @@
         <v>82</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -1783,7 +1783,7 @@
         <v>83</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -1791,7 +1791,7 @@
         <v>84</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -1799,7 +1799,7 @@
         <v>85</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -1807,7 +1807,7 @@
         <v>86</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -1815,7 +1815,7 @@
         <v>87</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -1823,7 +1823,7 @@
         <v>88</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -1831,7 +1831,7 @@
         <v>89</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -1839,7 +1839,7 @@
         <v>90</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -1847,7 +1847,7 @@
         <v>91</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -1855,7 +1855,7 @@
         <v>92</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -1863,7 +1863,7 @@
         <v>93</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -1871,7 +1871,7 @@
         <v>94</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -1879,7 +1879,7 @@
         <v>95</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -1887,7 +1887,7 @@
         <v>96</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -1895,7 +1895,7 @@
         <v>97</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -1903,7 +1903,7 @@
         <v>98</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -1911,7 +1911,7 @@
         <v>99</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -1919,7 +1919,7 @@
         <v>100</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -1927,7 +1927,7 @@
         <v>101</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -1935,7 +1935,7 @@
         <v>102</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -1943,7 +1943,7 @@
         <v>103</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -1951,7 +1951,7 @@
         <v>104</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -1959,7 +1959,7 @@
         <v>105</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -1967,7 +1967,7 @@
         <v>106</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -1975,7 +1975,7 @@
         <v>107</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -1983,7 +1983,7 @@
         <v>108</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -1991,7 +1991,7 @@
         <v>109</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -1999,7 +1999,7 @@
         <v>110</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2007,7 +2007,7 @@
         <v>111</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2015,7 +2015,7 @@
         <v>112</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2023,7 +2023,7 @@
         <v>113</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -2031,7 +2031,7 @@
         <v>114</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -2039,7 +2039,7 @@
         <v>115</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -2047,7 +2047,7 @@
         <v>116</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -2055,7 +2055,7 @@
         <v>117</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -2063,7 +2063,7 @@
         <v>118</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -2071,7 +2071,7 @@
         <v>119</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -2079,7 +2079,7 @@
         <v>120</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -2087,7 +2087,7 @@
         <v>121</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -2095,7 +2095,7 @@
         <v>122</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -2103,7 +2103,7 @@
         <v>123</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -2111,7 +2111,7 @@
         <v>124</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2125,7 @@
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A3" sqref="A3:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2192,57 +2192,57 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>